<commit_message>
Newest data is not great
But the improved data import and analysis I created in LoadAllData_New is much better, more robust, less prone to error, and easier to modify.
</commit_message>
<xml_diff>
--- a/BPA_Static_Characterization_Test/10mmData_Nov2022/CompareLoadData10mmColumns.xlsx
+++ b/BPA_Static_Characterization_Test/10mmData_Nov2022/CompareLoadData10mmColumns.xlsx
@@ -5,31 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\GitHub\Muscle_Sensory\BPA_Static_Characterization_Test\10mmData_Nov2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Muscle_Sensory\BPA_Static_Characterization_Test\10mmData_Nov2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4643317A-E3A5-4B69-A23D-B41DECFF62FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1B0393-2233-42B0-9D6D-62B063D46050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{73FEC325-17B2-4DAF-AC7C-7A8427CCB55B}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{73FEC325-17B2-4DAF-AC7C-7A8427CCB55B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -80,10 +69,10 @@
     <t>P/DP (1/2)</t>
   </si>
   <si>
-    <t>kink (length)</t>
-  </si>
-  <si>
     <t>kink (percentage)</t>
+  </si>
+  <si>
+    <t>length kindedd</t>
   </si>
 </sst>
 </file>
@@ -438,15 +427,15 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.109375" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -454,7 +443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -462,7 +451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -470,7 +459,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -478,7 +467,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -486,15 +475,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -502,15 +491,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -518,7 +507,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -526,7 +515,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -534,7 +523,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -542,7 +531,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -550,7 +539,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>5</v>
       </c>

</xml_diff>